<commit_message>
removed all files. Starting again.
</commit_message>
<xml_diff>
--- a/Research/literature_review.xlsx
+++ b/Research/literature_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g_gna\Documents\TCD\Modules\CS7CS5_Dissertation\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373C9501-1E27-40ED-996F-BB504AE78979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FACB377-DE1E-4CF0-A900-CD13A0FACEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9463" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Title</t>
   </si>
@@ -553,6 +553,16 @@
   </si>
   <si>
     <t>This work combines agent-based modeling of complex emergent systems and constructionism to design learning environments termed as an Emergent Systems Microworld (ESM), which with its consistent underlying rules regarding agent properties/behaviors, serve as an excellent experimental platform for learners to investigate different aspects of modeled phenomena through collective knowledge construction by engaging in scientific inquiry practices. The ESM design approach is based on restructuration theory which argues for the design and study of new representational forms for learning and expressing knowledge. Three studies were conducted that investigate how restructuration properties in ESM design supports student engagement in doing science by shaping and using scientific inquiry practices to learn about disciplinary ideas.</t>
+  </si>
+  <si>
+    <t># Microworlds need to be user friendly as complexity hinders learning. # Brief instructions must be given to novice users.</t>
+  </si>
+  <si>
+    <t>Web-Based Simulation Systems in Technological
+Education Implemented as Micro-Worlds</t>
+  </si>
+  <si>
+    <t>Microworld, Web, AJAX SVG, Education</t>
   </si>
 </sst>
 </file>
@@ -2410,13 +2420,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.75" x14ac:dyDescent="0.3"/>
@@ -2750,6 +2760,20 @@
       </c>
       <c r="K9" s="34" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2010</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding implementation and evaluation sections
</commit_message>
<xml_diff>
--- a/Research/literature_review.xlsx
+++ b/Research/literature_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g_gna\Documents\TCD\Modules\CS7CS5_Dissertation\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C1A796-77E9-4961-BBE6-1A7941BB510A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB2FA17-10DE-417C-82FD-F991909AC954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9463" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5352,7 +5352,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>